<commit_message>
test data and updated plotters
</commit_message>
<xml_diff>
--- a/Controller/controller_V3_matlab/customer_inputs_MX_BEND_0_DEG.xlsx
+++ b/Controller/controller_V3_matlab/customer_inputs_MX_BEND_0_DEG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tak/Documents/GitHub/ME-463-Can-Crusher/Controller/controller_V3_matlab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattl\Documents\Purdue\Fall 2025\ME 463\ME-463-Can-Crusher\Controller\controller_V3_matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEE9DBA-F6B8-2A4B-811E-F58DEDEB6952}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806107CD-94D3-4226-96EA-9C698603E0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" xr2:uid="{3A1ED538-D941-4692-8CDC-808B275BDBD0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3A1ED538-D941-4692-8CDC-808B275BDBD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Inputs" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Hold Time [s]</t>
   </si>
@@ -52,13 +63,16 @@
   </si>
   <si>
     <t>Bending [in-lbf]</t>
+  </si>
+  <si>
+    <t>Checkout Load</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,35 +531,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D38EA12-ABC1-4B15-987D-30F0BE17A6DB}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -555,34 +573,43 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3">
+        <v>800</v>
+      </c>
+      <c r="C3">
         <v>2342</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <f>976*12</f>
         <v>11712</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -592,34 +619,43 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
         <v>120</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>60</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="7">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7">
         <v>60</v>
       </c>
-      <c r="C7" s="7">
+      <c r="D7" s="7">
         <v>30</v>
       </c>
-      <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>